<commit_message>
Ajout function pour choisir le type de marker
</commit_message>
<xml_diff>
--- a/Beauce_Art_2014_2018.xlsx
+++ b/Beauce_Art_2014_2018.xlsx
@@ -389,9 +389,6 @@
     <t>-70.681361666667</t>
   </si>
   <si>
-    <t>Chaudierissimo – du fantastique, de la fantaisie et la Ch.</t>
-  </si>
-  <si>
     <t>Vortex</t>
   </si>
   <si>
@@ -890,6 +887,9 @@
   </si>
   <si>
     <t>-70.674408333333</t>
+  </si>
+  <si>
+    <t>Chaudierissimo – du fantastique, de la fantaisie et la Chaudière</t>
   </si>
 </sst>
 </file>
@@ -1245,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1919,23 +1919,23 @@
       <c r="B25" s="2">
         <v>2016</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="D25" t="s">
         <v>121</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>122</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" t="s">
         <v>125</v>
-      </c>
-      <c r="H25" t="s">
-        <v>126</v>
       </c>
       <c r="I25" t="s">
         <v>66</v>
@@ -1948,20 +1948,20 @@
       <c r="B26" s="2">
         <v>2016</v>
       </c>
-      <c r="C26" t="s">
-        <v>121</v>
+      <c r="C26" s="4" t="s">
+        <v>279</v>
       </c>
       <c r="D26" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" t="s">
         <v>127</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="H26" t="s">
         <v>42</v>
@@ -1977,23 +1977,23 @@
       <c r="B27" s="2">
         <v>2016</v>
       </c>
-      <c r="C27" t="s">
-        <v>121</v>
+      <c r="C27" s="4" t="s">
+        <v>279</v>
       </c>
       <c r="D27" t="s">
+        <v>130</v>
+      </c>
+      <c r="E27" t="s">
         <v>131</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="G27" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="H27" t="s">
         <v>134</v>
-      </c>
-      <c r="H27" t="s">
-        <v>135</v>
       </c>
       <c r="I27" t="s">
         <v>16</v>
@@ -2006,20 +2006,20 @@
       <c r="B28" s="2">
         <v>2016</v>
       </c>
-      <c r="C28" t="s">
-        <v>121</v>
+      <c r="C28" s="4" t="s">
+        <v>279</v>
       </c>
       <c r="D28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E28" t="s">
         <v>136</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="H28" t="s">
         <v>31</v>
@@ -2035,26 +2035,26 @@
       <c r="B29" s="2">
         <v>2016</v>
       </c>
-      <c r="C29" t="s">
-        <v>121</v>
+      <c r="C29" s="4" t="s">
+        <v>279</v>
       </c>
       <c r="D29" t="s">
+        <v>139</v>
+      </c>
+      <c r="E29" t="s">
         <v>140</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="H29" t="s">
         <v>143</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>144</v>
-      </c>
-      <c r="I29" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -2065,19 +2065,19 @@
         <v>2016</v>
       </c>
       <c r="C30" t="s">
-        <v>121</v>
+        <v>279</v>
       </c>
       <c r="D30" t="s">
+        <v>145</v>
+      </c>
+      <c r="E30" t="s">
         <v>146</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="H30" t="s">
         <v>71</v>
@@ -2094,22 +2094,22 @@
         <v>2016</v>
       </c>
       <c r="C31" t="s">
-        <v>121</v>
+        <v>279</v>
       </c>
       <c r="D31" t="s">
+        <v>149</v>
+      </c>
+      <c r="E31" t="s">
         <v>150</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="H31" t="s">
         <v>153</v>
-      </c>
-      <c r="H31" t="s">
-        <v>154</v>
       </c>
       <c r="I31" t="s">
         <v>66</v>
@@ -2123,25 +2123,25 @@
         <v>2016</v>
       </c>
       <c r="C32" t="s">
-        <v>121</v>
+        <v>279</v>
       </c>
       <c r="D32" t="s">
+        <v>154</v>
+      </c>
+      <c r="E32" t="s">
         <v>155</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="G32" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="H32" t="s">
         <v>158</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>159</v>
-      </c>
-      <c r="I32" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -2152,22 +2152,22 @@
         <v>2016</v>
       </c>
       <c r="C33" t="s">
-        <v>121</v>
+        <v>279</v>
       </c>
       <c r="D33" t="s">
+        <v>160</v>
+      </c>
+      <c r="E33" t="s">
         <v>161</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="G33" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="H33" t="s">
         <v>164</v>
-      </c>
-      <c r="H33" t="s">
-        <v>165</v>
       </c>
       <c r="I33" t="s">
         <v>16</v>
@@ -2184,16 +2184,16 @@
         <v>72</v>
       </c>
       <c r="D34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E34" t="s">
         <v>93</v>
       </c>
       <c r="F34" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="H34" t="s">
         <v>96</v>
@@ -2216,25 +2216,25 @@
         <v>2017</v>
       </c>
       <c r="C36" t="s">
+        <v>168</v>
+      </c>
+      <c r="D36" t="s">
         <v>169</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>170</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="G36" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="H36" t="s">
         <v>173</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>174</v>
-      </c>
-      <c r="I36" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -2245,19 +2245,19 @@
         <v>2017</v>
       </c>
       <c r="C37" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D37" t="s">
+        <v>175</v>
+      </c>
+      <c r="E37" t="s">
         <v>176</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="G37" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>179</v>
       </c>
       <c r="H37" t="s">
         <v>54</v>
@@ -2274,25 +2274,25 @@
         <v>2017</v>
       </c>
       <c r="C38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D38" t="s">
+        <v>179</v>
+      </c>
+      <c r="E38" t="s">
         <v>180</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="G38" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="H38" t="s">
         <v>183</v>
       </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>184</v>
-      </c>
-      <c r="I38" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -2303,22 +2303,22 @@
         <v>2017</v>
       </c>
       <c r="C39" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D39" t="s">
+        <v>185</v>
+      </c>
+      <c r="E39" t="s">
         <v>186</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="G39" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="H39" t="s">
         <v>189</v>
-      </c>
-      <c r="H39" t="s">
-        <v>190</v>
       </c>
       <c r="I39" t="s">
         <v>66</v>
@@ -2332,22 +2332,22 @@
         <v>2017</v>
       </c>
       <c r="C40" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D40" t="s">
+        <v>190</v>
+      </c>
+      <c r="E40" t="s">
         <v>191</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="G40" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="H40" t="s">
         <v>194</v>
-      </c>
-      <c r="H40" t="s">
-        <v>195</v>
       </c>
       <c r="I40" t="s">
         <v>16</v>
@@ -2361,22 +2361,22 @@
         <v>2017</v>
       </c>
       <c r="C41" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D41" t="s">
+        <v>195</v>
+      </c>
+      <c r="E41" t="s">
         <v>196</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="G41" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="H41" t="s">
         <v>199</v>
-      </c>
-      <c r="H41" t="s">
-        <v>200</v>
       </c>
       <c r="I41" t="s">
         <v>16</v>
@@ -2390,19 +2390,19 @@
         <v>2017</v>
       </c>
       <c r="C42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D42" t="s">
+        <v>200</v>
+      </c>
+      <c r="E42" t="s">
         <v>201</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="H42" t="s">
         <v>71</v>
@@ -2419,19 +2419,19 @@
         <v>2017</v>
       </c>
       <c r="C43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D43" t="s">
+        <v>204</v>
+      </c>
+      <c r="E43" t="s">
         <v>205</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="H43" t="s">
         <v>71</v>
@@ -2448,25 +2448,25 @@
         <v>2017</v>
       </c>
       <c r="C44" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D44" t="s">
+        <v>208</v>
+      </c>
+      <c r="E44" t="s">
         <v>209</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="G44" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="H44" t="s">
         <v>212</v>
       </c>
-      <c r="H44" t="s">
+      <c r="I44" t="s">
         <v>213</v>
-      </c>
-      <c r="I44" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
@@ -2477,25 +2477,25 @@
         <v>2017</v>
       </c>
       <c r="C45" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D45" t="s">
+        <v>214</v>
+      </c>
+      <c r="E45" t="s">
         <v>215</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="G45" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="H45" t="s">
         <v>218</v>
       </c>
-      <c r="H45" t="s">
+      <c r="I45" t="s">
         <v>219</v>
-      </c>
-      <c r="I45" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
@@ -2506,22 +2506,22 @@
         <v>2017</v>
       </c>
       <c r="C46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D46" t="s">
+        <v>220</v>
+      </c>
+      <c r="E46" t="s">
         <v>221</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="G46" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="H46" t="s">
         <v>224</v>
-      </c>
-      <c r="H46" t="s">
-        <v>225</v>
       </c>
       <c r="I46" t="s">
         <v>16</v>
@@ -2538,22 +2538,22 @@
         <v>2018</v>
       </c>
       <c r="C48" t="s">
+        <v>225</v>
+      </c>
+      <c r="D48" t="s">
         <v>226</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>227</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="G48" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="G48" s="3" t="s">
+      <c r="H48" t="s">
         <v>230</v>
-      </c>
-      <c r="H48" t="s">
-        <v>231</v>
       </c>
       <c r="I48" t="s">
         <v>16</v>
@@ -2567,25 +2567,25 @@
         <v>2018</v>
       </c>
       <c r="C49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D49" t="s">
+        <v>231</v>
+      </c>
+      <c r="E49" t="s">
         <v>232</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="G49" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="G49" s="3" t="s">
+      <c r="H49" t="s">
         <v>235</v>
       </c>
-      <c r="H49" t="s">
+      <c r="I49" t="s">
         <v>236</v>
-      </c>
-      <c r="I49" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
@@ -2596,25 +2596,25 @@
         <v>2018</v>
       </c>
       <c r="C50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D50" t="s">
+        <v>237</v>
+      </c>
+      <c r="E50" t="s">
         <v>238</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="H50" t="s">
         <v>239</v>
       </c>
-      <c r="F50" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="H50" t="s">
+      <c r="I50" t="s">
         <v>240</v>
-      </c>
-      <c r="I50" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
@@ -2625,19 +2625,19 @@
         <v>2018</v>
       </c>
       <c r="C51" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D51" t="s">
+        <v>241</v>
+      </c>
+      <c r="E51" t="s">
         <v>242</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="G51" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>245</v>
       </c>
       <c r="H51" t="s">
         <v>42</v>
@@ -2654,22 +2654,22 @@
         <v>2018</v>
       </c>
       <c r="C52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D52" t="s">
+        <v>245</v>
+      </c>
+      <c r="E52" t="s">
         <v>246</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="G52" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="G52" s="3" t="s">
+      <c r="H52" t="s">
         <v>249</v>
-      </c>
-      <c r="H52" t="s">
-        <v>250</v>
       </c>
       <c r="I52" t="s">
         <v>66</v>
@@ -2683,22 +2683,22 @@
         <v>2018</v>
       </c>
       <c r="C53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D53" t="s">
+        <v>250</v>
+      </c>
+      <c r="E53" t="s">
         <v>251</v>
       </c>
-      <c r="E53" t="s">
+      <c r="F53" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="G53" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="G53" s="3" t="s">
+      <c r="H53" t="s">
         <v>254</v>
-      </c>
-      <c r="H53" t="s">
-        <v>255</v>
       </c>
       <c r="I53" t="s">
         <v>112</v>
@@ -2712,25 +2712,25 @@
         <v>2018</v>
       </c>
       <c r="C54" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D54" t="s">
+        <v>255</v>
+      </c>
+      <c r="E54" t="s">
         <v>256</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="G54" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="G54" s="3" t="s">
-        <v>259</v>
-      </c>
       <c r="H54" t="s">
+        <v>183</v>
+      </c>
+      <c r="I54" t="s">
         <v>184</v>
-      </c>
-      <c r="I54" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
@@ -2741,22 +2741,22 @@
         <v>2018</v>
       </c>
       <c r="C55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D55" t="s">
+        <v>259</v>
+      </c>
+      <c r="E55" t="s">
         <v>260</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="G55" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="G55" s="3" t="s">
+      <c r="H55" t="s">
         <v>263</v>
-      </c>
-      <c r="H55" t="s">
-        <v>264</v>
       </c>
       <c r="I55" t="s">
         <v>16</v>
@@ -2770,25 +2770,25 @@
         <v>2018</v>
       </c>
       <c r="C56" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D56" t="s">
+        <v>264</v>
+      </c>
+      <c r="E56" t="s">
         <v>265</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="G56" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="H56" t="s">
         <v>268</v>
       </c>
-      <c r="H56" t="s">
+      <c r="I56" t="s">
         <v>269</v>
-      </c>
-      <c r="I56" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
@@ -2799,25 +2799,25 @@
         <v>2018</v>
       </c>
       <c r="C57" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D57" t="s">
+        <v>270</v>
+      </c>
+      <c r="E57" t="s">
         <v>271</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="G57" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="H57" t="s">
         <v>274</v>
       </c>
-      <c r="H57" t="s">
+      <c r="I57" t="s">
         <v>275</v>
-      </c>
-      <c r="I57" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
@@ -2828,19 +2828,19 @@
         <v>2018</v>
       </c>
       <c r="C58" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D58" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E58" t="s">
         <v>28</v>
       </c>
       <c r="F58" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G58" s="3" t="s">
         <v>278</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>279</v>
       </c>
       <c r="H58" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Update button pour recadrer
</commit_message>
<xml_diff>
--- a/Beauce_Art_2014_2018.xlsx
+++ b/Beauce_Art_2014_2018.xlsx
@@ -1245,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2064,7 +2064,7 @@
       <c r="B30" s="2">
         <v>2016</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="4" t="s">
         <v>279</v>
       </c>
       <c r="D30" t="s">
@@ -2093,7 +2093,7 @@
       <c r="B31" s="2">
         <v>2016</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="4" t="s">
         <v>279</v>
       </c>
       <c r="D31" t="s">
@@ -2122,7 +2122,7 @@
       <c r="B32" s="2">
         <v>2016</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="4" t="s">
         <v>279</v>
       </c>
       <c r="D32" t="s">
@@ -2151,7 +2151,7 @@
       <c r="B33" s="2">
         <v>2016</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="4" t="s">
         <v>279</v>
       </c>
       <c r="D33" t="s">

</xml_diff>